<commit_message>
Stop tracking INVESTMENT excel file
</commit_message>
<xml_diff>
--- a/CURRENT STATUS/Current_status_2025-08-27.xlsx
+++ b/CURRENT STATUS/Current_status_2025-08-27.xlsx
@@ -506,10 +506,10 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>45897</v>
+        <v>45895</v>
       </c>
       <c r="C2" t="n">
-        <v>87.15000000000001</v>
+        <v>86.59</v>
       </c>
       <c r="D2" t="n">
         <v>25</v>
@@ -518,10 +518,10 @@
         <v>49</v>
       </c>
       <c r="F2" t="n">
-        <v>85.60951761236039</v>
+        <v>85.48114408005708</v>
       </c>
       <c r="G2" t="n">
-        <v>84.85446690843563</v>
+        <v>84.75881969628711</v>
       </c>
       <c r="H2" t="n">
         <v>14</v>
@@ -530,7 +530,7 @@
         <v>39</v>
       </c>
       <c r="J2" t="n">
-        <v>62.49436607612628</v>
+        <v>59.17351827644686</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
@@ -550,10 +550,10 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>45897</v>
+        <v>45895</v>
       </c>
       <c r="C3" t="n">
-        <v>117.29</v>
+        <v>116.33</v>
       </c>
       <c r="D3" t="n">
         <v>8</v>
@@ -562,10 +562,10 @@
         <v>196</v>
       </c>
       <c r="F3" t="n">
-        <v>115.4173313131937</v>
+        <v>114.8822831169633</v>
       </c>
       <c r="G3" t="n">
-        <v>101.5686716007576</v>
+        <v>101.4074082968453</v>
       </c>
       <c r="H3" t="n">
         <v>5</v>
@@ -574,7 +574,7 @@
         <v>80</v>
       </c>
       <c r="J3" t="n">
-        <v>71.16295571349227</v>
+        <v>65.54654453288495</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
@@ -594,10 +594,10 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>45897</v>
+        <v>45895</v>
       </c>
       <c r="C4" t="n">
-        <v>47.81</v>
+        <v>48.25</v>
       </c>
       <c r="D4" t="n">
         <v>10</v>
@@ -606,10 +606,10 @@
         <v>48</v>
       </c>
       <c r="F4" t="n">
-        <v>48.72482219405865</v>
+        <v>48.92811601496058</v>
       </c>
       <c r="G4" t="n">
-        <v>49.30974213087918</v>
+        <v>49.37356094495915</v>
       </c>
       <c r="H4" t="n">
         <v>23</v>
@@ -618,7 +618,7 @@
         <v>47</v>
       </c>
       <c r="J4" t="n">
-        <v>40.66718141195588</v>
+        <v>42.90347922663884</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
@@ -638,10 +638,10 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>45897</v>
+        <v>45895</v>
       </c>
       <c r="C5" t="n">
-        <v>262.14</v>
+        <v>263.99</v>
       </c>
       <c r="D5" t="n">
         <v>25</v>
@@ -650,10 +650,10 @@
         <v>45</v>
       </c>
       <c r="F5" t="n">
-        <v>264.7241337368294</v>
+        <v>264.9394782148985</v>
       </c>
       <c r="G5" t="n">
-        <v>264.6164646065235</v>
+        <v>264.7290311795473</v>
       </c>
       <c r="H5" t="n">
         <v>16</v>
@@ -662,7 +662,7 @@
         <v>62</v>
       </c>
       <c r="J5" t="n">
-        <v>42.96757702172885</v>
+        <v>47.30924099333645</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
@@ -682,10 +682,10 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>45897</v>
+        <v>45895</v>
       </c>
       <c r="C6" t="n">
-        <v>88.11</v>
+        <v>88.56</v>
       </c>
       <c r="D6" t="n">
         <v>7</v>
@@ -694,10 +694,10 @@
         <v>73</v>
       </c>
       <c r="F6" t="n">
-        <v>89.2556174226649</v>
+        <v>89.63748989688654</v>
       </c>
       <c r="G6" t="n">
-        <v>90.80488163550429</v>
+        <v>90.87973945871273</v>
       </c>
       <c r="H6" t="n">
         <v>17</v>
@@ -706,7 +706,7 @@
         <v>41</v>
       </c>
       <c r="J6" t="n">
-        <v>29.97964340587372</v>
+        <v>32.06904172280153</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
@@ -726,10 +726,10 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>45897</v>
+        <v>45895</v>
       </c>
       <c r="C7" t="n">
-        <v>167.16</v>
+        <v>168.77</v>
       </c>
       <c r="D7" t="n">
         <v>15</v>
@@ -738,10 +738,10 @@
         <v>35</v>
       </c>
       <c r="F7" t="n">
-        <v>170.3174550945238</v>
+        <v>170.7685201080272</v>
       </c>
       <c r="G7" t="n">
-        <v>171.6775908491188</v>
+        <v>171.9433314873023</v>
       </c>
       <c r="H7" t="n">
         <v>30</v>
@@ -750,7 +750,7 @@
         <v>52</v>
       </c>
       <c r="J7" t="n">
-        <v>44.29995567836974</v>
+        <v>46.37145806981436</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
@@ -770,10 +770,10 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>45897</v>
+        <v>45895</v>
       </c>
       <c r="C8" t="n">
-        <v>21.62</v>
+        <v>21.79</v>
       </c>
       <c r="D8" t="n">
         <v>7</v>
@@ -782,10 +782,10 @@
         <v>60</v>
       </c>
       <c r="F8" t="n">
-        <v>21.88810260346938</v>
+        <v>21.97747013795918</v>
       </c>
       <c r="G8" t="n">
-        <v>21.89977051920662</v>
+        <v>21.9092542656204</v>
       </c>
       <c r="H8" t="n">
         <v>29</v>
@@ -794,7 +794,7 @@
         <v>46</v>
       </c>
       <c r="J8" t="n">
-        <v>46.23706664530066</v>
+        <v>48.23490240805658</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
@@ -803,7 +803,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>B_N_Y</t>
         </is>
       </c>
     </row>
@@ -814,10 +814,10 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>45897</v>
+        <v>45895</v>
       </c>
       <c r="C9" t="n">
-        <v>25.93</v>
+        <v>26.01</v>
       </c>
       <c r="D9" t="n">
         <v>5</v>
@@ -826,10 +826,10 @@
         <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>25.94248732808008</v>
+        <v>25.94873099212012</v>
       </c>
       <c r="G9" t="n">
-        <v>25.70529148794653</v>
+        <v>25.65535626304575</v>
       </c>
       <c r="H9" t="n">
         <v>13</v>
@@ -838,7 +838,7 @@
         <v>45</v>
       </c>
       <c r="J9" t="n">
-        <v>67.91704738442129</v>
+        <v>70.39893240239451</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
@@ -858,10 +858,10 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>45897</v>
+        <v>45895</v>
       </c>
       <c r="C10" t="n">
-        <v>59.57</v>
+        <v>60.04</v>
       </c>
       <c r="D10" t="n">
         <v>12</v>
@@ -870,10 +870,10 @@
         <v>72</v>
       </c>
       <c r="F10" t="n">
-        <v>59.51671457034555</v>
+        <v>59.50702631040837</v>
       </c>
       <c r="G10" t="n">
-        <v>59.09329180255705</v>
+        <v>59.07986340262906</v>
       </c>
       <c r="H10" t="n">
         <v>29</v>
@@ -882,7 +882,7 @@
         <v>48</v>
       </c>
       <c r="J10" t="n">
-        <v>52.03503024020654</v>
+        <v>54.49285588394612</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
@@ -902,10 +902,10 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>45897</v>
+        <v>45895</v>
       </c>
       <c r="C11" t="n">
-        <v>147.26</v>
+        <v>148.69</v>
       </c>
       <c r="D11" t="n">
         <v>13</v>
@@ -914,10 +914,10 @@
         <v>106</v>
       </c>
       <c r="F11" t="n">
-        <v>149.2099059052187</v>
+        <v>149.5348902227552</v>
       </c>
       <c r="G11" t="n">
-        <v>146.0475011084597</v>
+        <v>146.0244058914295</v>
       </c>
       <c r="H11" t="n">
         <v>14</v>
@@ -926,7 +926,7 @@
         <v>45</v>
       </c>
       <c r="J11" t="n">
-        <v>44.03065952930767</v>
+        <v>48.35756822698924</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
@@ -935,7 +935,7 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>B_N_Y</t>
         </is>
       </c>
     </row>
@@ -946,10 +946,10 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>45897</v>
+        <v>45895</v>
       </c>
       <c r="C12" t="n">
-        <v>202.89</v>
+        <v>202.49</v>
       </c>
       <c r="D12" t="n">
         <v>5</v>
@@ -958,10 +958,10 @@
         <v>164</v>
       </c>
       <c r="F12" t="n">
-        <v>202.8425307741511</v>
+        <v>202.8187961612267</v>
       </c>
       <c r="G12" t="n">
-        <v>187.7734392619444</v>
+        <v>187.5879599890849</v>
       </c>
       <c r="H12" t="n">
         <v>30</v>
@@ -970,7 +970,7 @@
         <v>52</v>
       </c>
       <c r="J12" t="n">
-        <v>58.74603509759331</v>
+        <v>58.34945619049549</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
@@ -990,10 +990,10 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>45897</v>
+        <v>45895</v>
       </c>
       <c r="C13" t="n">
-        <v>386.76</v>
+        <v>393</v>
       </c>
       <c r="D13" t="n">
         <v>5</v>
@@ -1002,10 +1002,10 @@
         <v>83</v>
       </c>
       <c r="F13" t="n">
-        <v>388.8742946898728</v>
+        <v>389.9314420348093</v>
       </c>
       <c r="G13" t="n">
-        <v>399.2804809008172</v>
+        <v>399.5858584837641</v>
       </c>
       <c r="H13" t="n">
         <v>2</v>
@@ -1014,7 +1014,7 @@
         <v>52</v>
       </c>
       <c r="J13" t="n">
-        <v>25.04604430082163</v>
+        <v>63.33395588756564</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
@@ -1034,10 +1034,10 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>45897</v>
+        <v>45895</v>
       </c>
       <c r="C14" t="n">
-        <v>29.18</v>
+        <v>29.38</v>
       </c>
       <c r="D14" t="n">
         <v>8</v>
@@ -1046,10 +1046,10 @@
         <v>56</v>
       </c>
       <c r="F14" t="n">
-        <v>29.75002421365132</v>
+        <v>29.91288827469454</v>
       </c>
       <c r="G14" t="n">
-        <v>29.85452501037364</v>
+        <v>29.87905319256971</v>
       </c>
       <c r="H14" t="n">
         <v>24</v>
@@ -1058,7 +1058,7 @@
         <v>44</v>
       </c>
       <c r="J14" t="n">
-        <v>42.97081687554697</v>
+        <v>44.57734174937318</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>B_N_Y</t>
         </is>
       </c>
     </row>
@@ -1078,10 +1078,10 @@
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>45897</v>
+        <v>45895</v>
       </c>
       <c r="C15" t="n">
-        <v>553.8</v>
+        <v>558.84</v>
       </c>
       <c r="D15" t="n">
         <v>12</v>
@@ -1090,10 +1090,10 @@
         <v>42</v>
       </c>
       <c r="F15" t="n">
-        <v>564.9377957815218</v>
+        <v>566.9628495599803</v>
       </c>
       <c r="G15" t="n">
-        <v>569.4925615128361</v>
+        <v>570.2580523183403</v>
       </c>
       <c r="H15" t="n">
         <v>22</v>
@@ -1102,7 +1102,7 @@
         <v>43</v>
       </c>
       <c r="J15" t="n">
-        <v>37.09354001388515</v>
+        <v>40.28750617781254</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>
@@ -1122,10 +1122,10 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>45897</v>
+        <v>45895</v>
       </c>
       <c r="C16" t="n">
-        <v>3304.9</v>
+        <v>3330.8</v>
       </c>
       <c r="D16" t="n">
         <v>64</v>
@@ -1134,10 +1134,10 @@
         <v>180</v>
       </c>
       <c r="F16" t="n">
-        <v>3184.683711371494</v>
+        <v>3180.867321256303</v>
       </c>
       <c r="G16" t="n">
-        <v>3015.354889970335</v>
+        <v>3012.119749076148</v>
       </c>
       <c r="H16" t="n">
         <v>7</v>
@@ -1146,7 +1146,7 @@
         <v>18</v>
       </c>
       <c r="J16" t="n">
-        <v>46.43532525254205</v>
+        <v>51.76562365762512</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
@@ -1166,10 +1166,10 @@
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>45897</v>
+        <v>45895</v>
       </c>
       <c r="C17" t="n">
-        <v>1966.6</v>
+        <v>2007.1</v>
       </c>
       <c r="D17" t="n">
         <v>22</v>
@@ -1178,10 +1178,10 @@
         <v>105</v>
       </c>
       <c r="F17" t="n">
-        <v>2063.265107129296</v>
+        <v>2072.471307808276</v>
       </c>
       <c r="G17" t="n">
-        <v>2206.699685569138</v>
+        <v>2211.316987214698</v>
       </c>
       <c r="H17" t="n">
         <v>5</v>
@@ -1190,7 +1190,7 @@
         <v>39</v>
       </c>
       <c r="J17" t="n">
-        <v>29.79723283813031</v>
+        <v>40.03153029554537</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>

</xml_diff>